<commit_message>
Teste Feito - So correr pro abraco!
</commit_message>
<xml_diff>
--- a/Razer.xlsx
+++ b/Razer.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="399">
-  <si>
-    <t>Treinamento</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="400">
   <si>
     <t>gostei de um vídeo do @youtube https://t.co/crmppi1hvn razer raiju ps4 pro controller review &amp;amp; unboxing</t>
   </si>
@@ -1283,12 +1280,18 @@
   <si>
     <t>gostei de um vídeo @youtube https://t.co/uwx7vtj0zz - comprei um full razer para jogar minecraft !!?</t>
   </si>
+  <si>
+    <t>definicao</t>
+  </si>
+  <si>
+    <t>treinamento</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1308,6 +1311,23 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1348,12 +1368,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1692,137 +1716,139 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B301"/>
+  <dimension ref="A1:F301"/>
   <sheetViews>
-    <sheetView topLeftCell="A275" workbookViewId="0">
-      <selection activeCell="B301" sqref="B301"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="124.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="B1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>14</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>15</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1830,7 +1856,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1838,7 +1864,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1846,7 +1872,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1854,7 +1880,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1862,7 +1888,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -1870,7 +1896,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -1878,7 +1904,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -1886,7 +1912,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -1894,7 +1920,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -1902,7 +1928,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -1910,7 +1936,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -1918,7 +1944,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -1926,7 +1952,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -1934,7 +1960,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -1942,7 +1968,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -1950,7 +1976,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -1958,7 +1984,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -1966,7 +1992,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -1974,7 +2000,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -1982,7 +2008,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -1990,7 +2016,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -1998,7 +2024,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -2006,7 +2032,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -2014,7 +2040,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -2022,7 +2048,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -2030,7 +2056,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -2038,7 +2064,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -2046,7 +2072,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -2054,7 +2080,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -2062,7 +2088,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -2070,7 +2096,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -2078,7 +2104,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -2086,7 +2112,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -2094,7 +2120,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -2102,7 +2128,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -2110,7 +2136,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -2118,7 +2144,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -2126,7 +2152,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -2134,7 +2160,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -2142,7 +2168,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -2150,7 +2176,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -2158,7 +2184,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -2166,7 +2192,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -2174,7 +2200,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -2182,7 +2208,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -2190,7 +2216,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B62">
         <v>1</v>
@@ -2198,7 +2224,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -2206,7 +2232,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -2214,7 +2240,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -2222,7 +2248,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -2230,7 +2256,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -2238,7 +2264,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B68">
         <v>1</v>
@@ -2246,7 +2272,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -2254,7 +2280,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -2262,7 +2288,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B71">
         <v>1</v>
@@ -2270,7 +2296,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -2278,7 +2304,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -2286,7 +2312,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -2294,7 +2320,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -2302,7 +2328,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -2310,7 +2336,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -2318,7 +2344,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B78">
         <v>1</v>
@@ -2326,7 +2352,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -2334,7 +2360,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B80">
         <v>1</v>
@@ -2342,7 +2368,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -2350,7 +2376,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B82">
         <v>1</v>
@@ -2358,7 +2384,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B83">
         <v>1</v>
@@ -2366,7 +2392,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -2374,7 +2400,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B85">
         <v>0</v>
@@ -2382,7 +2408,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -2390,7 +2416,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -2398,7 +2424,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -2406,7 +2432,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -2414,7 +2440,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B90">
         <v>1</v>
@@ -2422,7 +2448,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B91">
         <v>1</v>
@@ -2430,7 +2456,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B92">
         <v>1</v>
@@ -2438,7 +2464,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B93">
         <v>1</v>
@@ -2446,7 +2472,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B94">
         <v>1</v>
@@ -2454,7 +2480,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B95">
         <v>1</v>
@@ -2462,7 +2488,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -2470,7 +2496,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B97">
         <v>0</v>
@@ -2478,7 +2504,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B98">
         <v>0</v>
@@ -2486,7 +2512,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B99">
         <v>1</v>
@@ -2494,7 +2520,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B100">
         <v>1</v>
@@ -2502,7 +2528,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B101">
         <v>1</v>
@@ -2510,7 +2536,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B102">
         <v>0</v>
@@ -2518,7 +2544,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B103">
         <v>0</v>
@@ -2526,7 +2552,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B104">
         <v>1</v>
@@ -2534,7 +2560,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B105">
         <v>1</v>
@@ -2542,7 +2568,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B106">
         <v>1</v>
@@ -2550,7 +2576,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B107">
         <v>1</v>
@@ -2558,7 +2584,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B108">
         <v>1</v>
@@ -2566,7 +2592,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B109">
         <v>1</v>
@@ -2574,7 +2600,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B110">
         <v>1</v>
@@ -2582,7 +2608,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B111">
         <v>0</v>
@@ -2590,7 +2616,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B112">
         <v>0</v>
@@ -2598,7 +2624,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B113">
         <v>0</v>
@@ -2606,7 +2632,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B114">
         <v>1</v>
@@ -2614,7 +2640,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B115">
         <v>1</v>
@@ -2622,7 +2648,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B116">
         <v>1</v>
@@ -2630,7 +2656,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B117">
         <v>1</v>
@@ -2638,7 +2664,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B118">
         <v>1</v>
@@ -2646,7 +2672,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B119">
         <v>0</v>
@@ -2654,7 +2680,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B120">
         <v>1</v>
@@ -2662,7 +2688,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B121">
         <v>1</v>
@@ -2670,7 +2696,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B122">
         <v>0</v>
@@ -2678,7 +2704,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B123">
         <v>1</v>
@@ -2686,7 +2712,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B124">
         <v>0</v>
@@ -2694,7 +2720,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B125">
         <v>0</v>
@@ -2702,7 +2728,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B126">
         <v>0</v>
@@ -2710,7 +2736,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B127">
         <v>0</v>
@@ -2718,7 +2744,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B128">
         <v>1</v>
@@ -2726,7 +2752,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B129">
         <v>0</v>
@@ -2734,7 +2760,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B130">
         <v>1</v>
@@ -2742,7 +2768,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B131">
         <v>0</v>
@@ -2750,7 +2776,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B132">
         <v>1</v>
@@ -2758,7 +2784,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B133">
         <v>1</v>
@@ -2766,7 +2792,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B134">
         <v>1</v>
@@ -2774,7 +2800,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B135">
         <v>1</v>
@@ -2782,7 +2808,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B136">
         <v>1</v>
@@ -2790,7 +2816,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B137">
         <v>0</v>
@@ -2798,7 +2824,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B138">
         <v>1</v>
@@ -2806,7 +2832,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B139">
         <v>1</v>
@@ -2814,7 +2840,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B140">
         <v>0</v>
@@ -2822,7 +2848,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B141">
         <v>1</v>
@@ -2830,7 +2856,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B142">
         <v>1</v>
@@ -2838,7 +2864,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B143">
         <v>1</v>
@@ -2846,7 +2872,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B144">
         <v>0</v>
@@ -2854,7 +2880,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B145">
         <v>1</v>
@@ -2862,7 +2888,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B146">
         <v>1</v>
@@ -2870,7 +2896,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B147">
         <v>1</v>
@@ -2878,7 +2904,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B148">
         <v>1</v>
@@ -2886,7 +2912,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B149">
         <v>0</v>
@@ -2894,7 +2920,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B150">
         <v>1</v>
@@ -2902,7 +2928,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B151">
         <v>1</v>
@@ -2910,7 +2936,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B152">
         <v>0</v>
@@ -2918,7 +2944,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B153">
         <v>1</v>
@@ -2926,7 +2952,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B154">
         <v>1</v>
@@ -2934,7 +2960,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B155">
         <v>0</v>
@@ -2942,7 +2968,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B156">
         <v>0</v>
@@ -2950,7 +2976,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B157">
         <v>1</v>
@@ -2958,7 +2984,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B158">
         <v>0</v>
@@ -2966,7 +2992,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B159">
         <v>1</v>
@@ -2974,7 +3000,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B160">
         <v>0</v>
@@ -2982,7 +3008,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B161">
         <v>0</v>
@@ -2990,7 +3016,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B162">
         <v>1</v>
@@ -2998,7 +3024,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B163">
         <v>0</v>
@@ -3006,7 +3032,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B164">
         <v>1</v>
@@ -3014,7 +3040,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B165">
         <v>1</v>
@@ -3022,7 +3048,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B166">
         <v>0</v>
@@ -3030,7 +3056,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B167">
         <v>0</v>
@@ -3038,7 +3064,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B168">
         <v>0</v>
@@ -3046,7 +3072,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B169">
         <v>1</v>
@@ -3054,7 +3080,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B170">
         <v>0</v>
@@ -3062,7 +3088,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B171">
         <v>1</v>
@@ -3070,7 +3096,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B172">
         <v>0</v>
@@ -3078,7 +3104,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B173">
         <v>1</v>
@@ -3086,7 +3112,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B174">
         <v>1</v>
@@ -3094,7 +3120,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B175">
         <v>1</v>
@@ -3102,7 +3128,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B176">
         <v>1</v>
@@ -3110,7 +3136,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B177">
         <v>0</v>
@@ -3118,7 +3144,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B178">
         <v>1</v>
@@ -3126,7 +3152,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B179">
         <v>1</v>
@@ -3134,7 +3160,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B180">
         <v>1</v>
@@ -3142,7 +3168,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B181">
         <v>1</v>
@@ -3150,7 +3176,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B182">
         <v>1</v>
@@ -3158,7 +3184,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B183">
         <v>1</v>
@@ -3166,7 +3192,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B184">
         <v>1</v>
@@ -3174,7 +3200,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B185">
         <v>1</v>
@@ -3182,7 +3208,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B186">
         <v>0</v>
@@ -3190,7 +3216,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B187">
         <v>1</v>
@@ -3198,7 +3224,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B188">
         <v>1</v>
@@ -3206,7 +3232,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B189">
         <v>1</v>
@@ -3214,7 +3240,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B190">
         <v>1</v>
@@ -3222,7 +3248,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B191">
         <v>1</v>
@@ -3230,7 +3256,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B192">
         <v>1</v>
@@ -3238,7 +3264,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B193">
         <v>0</v>
@@ -3246,7 +3272,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B194">
         <v>1</v>
@@ -3254,7 +3280,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B195">
         <v>1</v>
@@ -3262,7 +3288,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B196">
         <v>0</v>
@@ -3270,7 +3296,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B197">
         <v>0</v>
@@ -3278,7 +3304,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B198">
         <v>0</v>
@@ -3286,7 +3312,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B199">
         <v>0</v>
@@ -3294,7 +3320,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B200">
         <v>1</v>
@@ -3302,7 +3328,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B201">
         <v>1</v>
@@ -3310,7 +3336,7 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B202">
         <v>1</v>
@@ -3318,7 +3344,7 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B203">
         <v>1</v>
@@ -3326,7 +3352,7 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B204">
         <v>1</v>
@@ -3334,7 +3360,7 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B205">
         <v>1</v>
@@ -3342,7 +3368,7 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B206">
         <v>0</v>
@@ -3350,7 +3376,7 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B207">
         <v>0</v>
@@ -3358,7 +3384,7 @@
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B208">
         <v>1</v>
@@ -3366,7 +3392,7 @@
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B209">
         <v>1</v>
@@ -3374,7 +3400,7 @@
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B210">
         <v>1</v>
@@ -3382,7 +3408,7 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B211">
         <v>1</v>
@@ -3390,7 +3416,7 @@
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B212">
         <v>0</v>
@@ -3398,7 +3424,7 @@
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B213">
         <v>0</v>
@@ -3406,7 +3432,7 @@
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B214">
         <v>0</v>
@@ -3414,7 +3440,7 @@
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B215">
         <v>0</v>
@@ -3422,7 +3448,7 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B216">
         <v>1</v>
@@ -3430,7 +3456,7 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B217">
         <v>1</v>
@@ -3438,7 +3464,7 @@
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B218">
         <v>1</v>
@@ -3446,7 +3472,7 @@
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B219">
         <v>0</v>
@@ -3454,7 +3480,7 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B220">
         <v>1</v>
@@ -3462,7 +3488,7 @@
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B221">
         <v>1</v>
@@ -3470,7 +3496,7 @@
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B222">
         <v>1</v>
@@ -3478,7 +3504,7 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B223">
         <v>0</v>
@@ -3486,7 +3512,7 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B224">
         <v>0</v>
@@ -3494,7 +3520,7 @@
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B225">
         <v>1</v>
@@ -3502,7 +3528,7 @@
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B226">
         <v>1</v>
@@ -3510,7 +3536,7 @@
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B227">
         <v>1</v>
@@ -3518,7 +3544,7 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B228">
         <v>1</v>
@@ -3526,7 +3552,7 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B229">
         <v>1</v>
@@ -3534,7 +3560,7 @@
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B230">
         <v>1</v>
@@ -3542,7 +3568,7 @@
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B231">
         <v>0</v>
@@ -3550,7 +3576,7 @@
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B232">
         <v>0</v>
@@ -3558,7 +3584,7 @@
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B233">
         <v>1</v>
@@ -3566,7 +3592,7 @@
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B234">
         <v>0</v>
@@ -3574,7 +3600,7 @@
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B235">
         <v>1</v>
@@ -3582,7 +3608,7 @@
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B236">
         <v>1</v>
@@ -3590,7 +3616,7 @@
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B237">
         <v>1</v>
@@ -3598,7 +3624,7 @@
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B238">
         <v>1</v>
@@ -3606,7 +3632,7 @@
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B239">
         <v>1</v>
@@ -3614,7 +3640,7 @@
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B240">
         <v>1</v>
@@ -3622,7 +3648,7 @@
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B241">
         <v>1</v>
@@ -3630,7 +3656,7 @@
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B242">
         <v>0</v>
@@ -3638,7 +3664,7 @@
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B243">
         <v>1</v>
@@ -3646,7 +3672,7 @@
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B244">
         <v>1</v>
@@ -3654,7 +3680,7 @@
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B245">
         <v>0</v>
@@ -3662,7 +3688,7 @@
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B246">
         <v>1</v>
@@ -3670,7 +3696,7 @@
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B247">
         <v>1</v>
@@ -3678,7 +3704,7 @@
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B248">
         <v>1</v>
@@ -3686,7 +3712,7 @@
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B249">
         <v>0</v>
@@ -3694,7 +3720,7 @@
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B250">
         <v>1</v>
@@ -3702,7 +3728,7 @@
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B251">
         <v>1</v>
@@ -3710,7 +3736,7 @@
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B252">
         <v>1</v>
@@ -3718,7 +3744,7 @@
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B253">
         <v>1</v>
@@ -3726,7 +3752,7 @@
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B254">
         <v>1</v>
@@ -3734,7 +3760,7 @@
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B255">
         <v>1</v>
@@ -3742,7 +3768,7 @@
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B256">
         <v>1</v>
@@ -3750,7 +3776,7 @@
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B257">
         <v>0</v>
@@ -3758,7 +3784,7 @@
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B258">
         <v>1</v>
@@ -3766,7 +3792,7 @@
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B259">
         <v>1</v>
@@ -3774,7 +3800,7 @@
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B260">
         <v>1</v>
@@ -3782,7 +3808,7 @@
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B261">
         <v>0</v>
@@ -3790,7 +3816,7 @@
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B262">
         <v>0</v>
@@ -3798,7 +3824,7 @@
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B263">
         <v>1</v>
@@ -3806,7 +3832,7 @@
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B264">
         <v>0</v>
@@ -3814,7 +3840,7 @@
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B265">
         <v>1</v>
@@ -3822,7 +3848,7 @@
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B266">
         <v>1</v>
@@ -3830,7 +3856,7 @@
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B267">
         <v>1</v>
@@ -3838,7 +3864,7 @@
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B268">
         <v>0</v>
@@ -3846,7 +3872,7 @@
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B269">
         <v>0</v>
@@ -3854,7 +3880,7 @@
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B270">
         <v>1</v>
@@ -3862,7 +3888,7 @@
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B271">
         <v>1</v>
@@ -3870,7 +3896,7 @@
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B272">
         <v>1</v>
@@ -3878,7 +3904,7 @@
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B273">
         <v>1</v>
@@ -3886,7 +3912,7 @@
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B274">
         <v>1</v>
@@ -3894,7 +3920,7 @@
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B275">
         <v>0</v>
@@ -3902,7 +3928,7 @@
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B276">
         <v>0</v>
@@ -3910,7 +3936,7 @@
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B277">
         <v>0</v>
@@ -3918,7 +3944,7 @@
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B278">
         <v>1</v>
@@ -3926,7 +3952,7 @@
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B279">
         <v>1</v>
@@ -3934,7 +3960,7 @@
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B280">
         <v>1</v>
@@ -3942,7 +3968,7 @@
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B281">
         <v>1</v>
@@ -3950,7 +3976,7 @@
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B282">
         <v>0</v>
@@ -3958,7 +3984,7 @@
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B283">
         <v>0</v>
@@ -3966,7 +3992,7 @@
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B284">
         <v>0</v>
@@ -3974,7 +4000,7 @@
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B285">
         <v>1</v>
@@ -3982,7 +4008,7 @@
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B286">
         <v>1</v>
@@ -3990,7 +4016,7 @@
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B287">
         <v>1</v>
@@ -3998,7 +4024,7 @@
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B288">
         <v>1</v>
@@ -4006,7 +4032,7 @@
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B289">
         <v>0</v>
@@ -4014,7 +4040,7 @@
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B290">
         <v>1</v>
@@ -4022,7 +4048,7 @@
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B291">
         <v>0</v>
@@ -4030,7 +4056,7 @@
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B292">
         <v>1</v>
@@ -4038,7 +4064,7 @@
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B293">
         <v>1</v>
@@ -4046,7 +4072,7 @@
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B294">
         <v>1</v>
@@ -4054,7 +4080,7 @@
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B295">
         <v>0</v>
@@ -4062,7 +4088,7 @@
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B296">
         <v>1</v>
@@ -4070,7 +4096,7 @@
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B297">
         <v>1</v>
@@ -4078,7 +4104,7 @@
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B298">
         <v>1</v>
@@ -4086,7 +4112,7 @@
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B299">
         <v>0</v>
@@ -4094,7 +4120,7 @@
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B300">
         <v>0</v>
@@ -4102,7 +4128,7 @@
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B301">
         <v>1</v>
@@ -4113,6 +4139,7 @@
     <hyperlink ref="A114" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4120,7 +4147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+    <sheetView topLeftCell="A127" workbookViewId="0">
       <selection activeCell="B201" sqref="B201"/>
     </sheetView>
   </sheetViews>
@@ -4131,12 +4158,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -4144,7 +4171,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -4152,7 +4179,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -4160,7 +4187,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -4168,7 +4195,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -4176,7 +4203,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -4184,7 +4211,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -4192,7 +4219,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -4200,7 +4227,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -4208,7 +4235,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -4216,7 +4243,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -4224,7 +4251,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -4232,7 +4259,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -4240,7 +4267,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -4248,7 +4275,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -4256,7 +4283,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -4264,7 +4291,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -4272,7 +4299,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -4280,7 +4307,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -4288,7 +4315,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -4296,7 +4323,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -4304,7 +4331,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -4312,7 +4339,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -4320,7 +4347,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -4328,7 +4355,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -4336,7 +4363,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -4344,7 +4371,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -4352,7 +4379,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -4360,7 +4387,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -4368,7 +4395,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -4376,7 +4403,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -4384,7 +4411,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -4392,7 +4419,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -4400,7 +4427,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -4408,7 +4435,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -4416,7 +4443,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -4424,7 +4451,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -4432,7 +4459,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -4440,7 +4467,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -4448,7 +4475,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -4456,7 +4483,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -4464,7 +4491,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -4472,7 +4499,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -4480,7 +4507,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -4488,7 +4515,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -4496,7 +4523,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -4504,7 +4531,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -4512,7 +4539,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -4520,7 +4547,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -4528,7 +4555,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -4536,7 +4563,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -4544,7 +4571,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -4552,7 +4579,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -4560,7 +4587,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -4568,7 +4595,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -4576,7 +4603,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B57">
         <v>1</v>
@@ -4584,7 +4611,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -4592,7 +4619,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -4600,7 +4627,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -4608,7 +4635,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -4616,7 +4643,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -4624,7 +4651,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -4632,7 +4659,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -4640,7 +4667,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -4648,7 +4675,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -4656,7 +4683,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -4664,7 +4691,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B68">
         <v>1</v>
@@ -4672,7 +4699,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -4680,7 +4707,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -4688,7 +4715,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -4696,7 +4723,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -4704,7 +4731,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -4712,7 +4739,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -4720,7 +4747,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -4728,7 +4755,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -4736,7 +4763,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -4744,7 +4771,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -4752,7 +4779,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -4760,7 +4787,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B80">
         <v>1</v>
@@ -4768,7 +4795,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -4776,7 +4803,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -4784,7 +4811,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B83">
         <v>1</v>
@@ -4792,7 +4819,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -4800,7 +4827,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -4808,7 +4835,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -4816,7 +4843,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -4824,7 +4851,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -4832,7 +4859,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -4840,7 +4867,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B90">
         <v>1</v>
@@ -4848,7 +4875,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B91">
         <v>1</v>
@@ -4856,7 +4883,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B92">
         <v>0</v>
@@ -4864,7 +4891,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B93">
         <v>1</v>
@@ -4872,7 +4899,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B94">
         <v>1</v>
@@ -4880,7 +4907,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B95">
         <v>1</v>
@@ -4888,7 +4915,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B96">
         <v>1</v>
@@ -4896,7 +4923,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B97">
         <v>1</v>
@@ -4904,7 +4931,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B98">
         <v>1</v>
@@ -4912,7 +4939,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -4920,7 +4947,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B100">
         <v>1</v>
@@ -4928,7 +4955,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B101">
         <v>1</v>
@@ -4936,7 +4963,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B102">
         <v>0</v>
@@ -4944,7 +4971,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B103">
         <v>1</v>
@@ -4952,7 +4979,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B104">
         <v>1</v>
@@ -4960,7 +4987,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B105">
         <v>1</v>
@@ -4968,7 +4995,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B106">
         <v>0</v>
@@ -4976,7 +5003,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B107">
         <v>1</v>
@@ -4984,7 +5011,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B108">
         <v>1</v>
@@ -4992,7 +5019,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B109">
         <v>1</v>
@@ -5000,7 +5027,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B110">
         <v>1</v>
@@ -5008,7 +5035,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B111">
         <v>0</v>
@@ -5016,7 +5043,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B112">
         <v>1</v>
@@ -5024,7 +5051,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B113">
         <v>0</v>
@@ -5032,7 +5059,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B114">
         <v>1</v>
@@ -5040,7 +5067,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B115">
         <v>1</v>
@@ -5048,7 +5075,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B116">
         <v>1</v>
@@ -5056,7 +5083,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B117">
         <v>1</v>
@@ -5064,7 +5091,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B118">
         <v>1</v>
@@ -5072,7 +5099,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B119">
         <v>1</v>
@@ -5080,7 +5107,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B120">
         <v>1</v>
@@ -5088,7 +5115,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B121">
         <v>1</v>
@@ -5096,7 +5123,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B122">
         <v>0</v>
@@ -5104,7 +5131,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B123">
         <v>1</v>
@@ -5112,7 +5139,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B124">
         <v>1</v>
@@ -5120,7 +5147,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B125">
         <v>1</v>
@@ -5128,7 +5155,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B126">
         <v>0</v>
@@ -5136,7 +5163,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B127">
         <v>1</v>
@@ -5144,7 +5171,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B128">
         <v>1</v>
@@ -5152,7 +5179,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B129">
         <v>1</v>
@@ -5160,7 +5187,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B130">
         <v>0</v>
@@ -5168,7 +5195,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B131">
         <v>1</v>
@@ -5176,7 +5203,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B132">
         <v>1</v>
@@ -5184,7 +5211,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B133">
         <v>1</v>
@@ -5192,7 +5219,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B134">
         <v>1</v>
@@ -5200,7 +5227,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B135">
         <v>1</v>
@@ -5208,7 +5235,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B136">
         <v>1</v>
@@ -5216,7 +5243,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B137">
         <v>1</v>
@@ -5224,7 +5251,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B138">
         <v>1</v>
@@ -5232,7 +5259,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B139">
         <v>1</v>
@@ -5240,7 +5267,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B140">
         <v>1</v>
@@ -5248,7 +5275,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B141">
         <v>1</v>
@@ -5256,7 +5283,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B142">
         <v>0</v>
@@ -5264,7 +5291,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B143">
         <v>0</v>
@@ -5272,7 +5299,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B144">
         <v>1</v>
@@ -5280,7 +5307,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B145">
         <v>1</v>
@@ -5288,7 +5315,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B146">
         <v>1</v>
@@ -5296,7 +5323,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B147">
         <v>0</v>
@@ -5304,7 +5331,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B148">
         <v>1</v>
@@ -5312,7 +5339,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B149">
         <v>1</v>
@@ -5320,7 +5347,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B150">
         <v>1</v>
@@ -5328,7 +5355,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B151">
         <v>1</v>
@@ -5336,7 +5363,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B152">
         <v>1</v>
@@ -5344,7 +5371,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B153">
         <v>1</v>
@@ -5352,7 +5379,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B154">
         <v>0</v>
@@ -5360,7 +5387,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B155">
         <v>1</v>
@@ -5368,7 +5395,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B156">
         <v>1</v>
@@ -5376,7 +5403,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B157">
         <v>1</v>
@@ -5384,7 +5411,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B158">
         <v>1</v>
@@ -5392,7 +5419,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B159">
         <v>1</v>
@@ -5400,7 +5427,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B160">
         <v>1</v>
@@ -5408,7 +5435,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B161">
         <v>0</v>
@@ -5416,7 +5443,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B162">
         <v>0</v>
@@ -5424,7 +5451,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B163">
         <v>1</v>
@@ -5432,7 +5459,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B164">
         <v>1</v>
@@ -5440,7 +5467,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B165">
         <v>1</v>
@@ -5448,7 +5475,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B166">
         <v>0</v>
@@ -5456,7 +5483,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B167">
         <v>1</v>
@@ -5464,7 +5491,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B168">
         <v>1</v>
@@ -5472,7 +5499,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B169">
         <v>1</v>
@@ -5480,7 +5507,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B170">
         <v>1</v>
@@ -5488,7 +5515,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B171">
         <v>0</v>
@@ -5496,7 +5523,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B172">
         <v>1</v>
@@ -5504,7 +5531,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B173">
         <v>1</v>
@@ -5512,7 +5539,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B174">
         <v>1</v>
@@ -5520,7 +5547,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B175">
         <v>1</v>
@@ -5528,7 +5555,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B176">
         <v>0</v>
@@ -5536,7 +5563,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B177">
         <v>0</v>
@@ -5544,7 +5571,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B178">
         <v>1</v>
@@ -5552,7 +5579,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B179">
         <v>0</v>
@@ -5560,7 +5587,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B180">
         <v>1</v>
@@ -5568,7 +5595,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B181">
         <v>1</v>
@@ -5576,7 +5603,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B182">
         <v>0</v>
@@ -5584,7 +5611,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B183">
         <v>1</v>
@@ -5592,7 +5619,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B184">
         <v>1</v>
@@ -5600,7 +5627,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B185">
         <v>0</v>
@@ -5608,7 +5635,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B186">
         <v>0</v>
@@ -5616,7 +5643,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B187">
         <v>1</v>
@@ -5624,7 +5651,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B188">
         <v>1</v>
@@ -5632,7 +5659,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B189">
         <v>1</v>
@@ -5640,7 +5667,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B190">
         <v>1</v>
@@ -5648,7 +5675,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B191">
         <v>1</v>
@@ -5656,7 +5683,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B192">
         <v>1</v>
@@ -5664,7 +5691,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B193">
         <v>0</v>
@@ -5672,7 +5699,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B194">
         <v>1</v>
@@ -5680,7 +5707,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B195">
         <v>1</v>
@@ -5688,7 +5715,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B196">
         <v>0</v>
@@ -5696,7 +5723,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B197">
         <v>1</v>
@@ -5704,7 +5731,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B198">
         <v>1</v>
@@ -5712,7 +5739,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B199">
         <v>1</v>
@@ -5720,7 +5747,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B200">
         <v>1</v>
@@ -5728,7 +5755,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B201">
         <v>1</v>

</xml_diff>

<commit_message>
Teste feito, Agora é correr pro abraco!
</commit_message>
<xml_diff>
--- a/Razer.xlsx
+++ b/Razer.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -1368,7 +1368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1377,6 +1377,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1718,7 +1721,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1737,8 +1742,8 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="B2" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1770,7 +1775,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1778,7 +1783,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="3"/>
     </row>
@@ -1795,7 +1800,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1803,7 +1808,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1843,7 +1848,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1859,7 +1864,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -1867,7 +1872,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -1875,7 +1880,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -1955,7 +1960,7 @@
         <v>26</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -1979,7 +1984,7 @@
         <v>29</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -2019,7 +2024,7 @@
         <v>31</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -2067,7 +2072,7 @@
         <v>35</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -2107,7 +2112,7 @@
         <v>38</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -2187,7 +2192,7 @@
         <v>44</v>
       </c>
       <c r="B58">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -2195,7 +2200,7 @@
         <v>45</v>
       </c>
       <c r="B59">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -2211,7 +2216,7 @@
         <v>47</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
@@ -2227,7 +2232,7 @@
         <v>48</v>
       </c>
       <c r="B63">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
@@ -2235,7 +2240,7 @@
         <v>49</v>
       </c>
       <c r="B64">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
@@ -2243,7 +2248,7 @@
         <v>50</v>
       </c>
       <c r="B65">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
@@ -2331,7 +2336,7 @@
         <v>60</v>
       </c>
       <c r="B76">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
@@ -2347,7 +2352,7 @@
         <v>62</v>
       </c>
       <c r="B78">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
@@ -2355,7 +2360,7 @@
         <v>63</v>
       </c>
       <c r="B79">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
@@ -2427,7 +2432,7 @@
         <v>70</v>
       </c>
       <c r="B88">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
@@ -2475,7 +2480,7 @@
         <v>74</v>
       </c>
       <c r="B94">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
@@ -2523,7 +2528,7 @@
         <v>79</v>
       </c>
       <c r="B100">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
@@ -2579,7 +2584,7 @@
         <v>84</v>
       </c>
       <c r="B107">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
@@ -2587,7 +2592,7 @@
         <v>85</v>
       </c>
       <c r="B108">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
@@ -2603,7 +2608,7 @@
         <v>87</v>
       </c>
       <c r="B110">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
@@ -2611,7 +2616,7 @@
         <v>88</v>
       </c>
       <c r="B111">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
@@ -2627,7 +2632,7 @@
         <v>90</v>
       </c>
       <c r="B113">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
@@ -2667,7 +2672,7 @@
         <v>93</v>
       </c>
       <c r="B118">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
@@ -2707,7 +2712,7 @@
         <v>96</v>
       </c>
       <c r="B123">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
@@ -2715,7 +2720,7 @@
         <v>97</v>
       </c>
       <c r="B124">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
@@ -2763,7 +2768,7 @@
         <v>102</v>
       </c>
       <c r="B130">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
@@ -2787,7 +2792,7 @@
         <v>105</v>
       </c>
       <c r="B133">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
@@ -2835,7 +2840,7 @@
         <v>109</v>
       </c>
       <c r="B139">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
@@ -2843,7 +2848,7 @@
         <v>110</v>
       </c>
       <c r="B140">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
@@ -2867,7 +2872,7 @@
         <v>113</v>
       </c>
       <c r="B143">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
@@ -2883,7 +2888,7 @@
         <v>115</v>
       </c>
       <c r="B145">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
@@ -2899,7 +2904,7 @@
         <v>116</v>
       </c>
       <c r="B147">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
@@ -2915,7 +2920,7 @@
         <v>117</v>
       </c>
       <c r="B149">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
@@ -2955,7 +2960,7 @@
         <v>120</v>
       </c>
       <c r="B154">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
@@ -2987,7 +2992,7 @@
         <v>123</v>
       </c>
       <c r="B158">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
@@ -2995,7 +3000,7 @@
         <v>124</v>
       </c>
       <c r="B159">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
@@ -3067,7 +3072,7 @@
         <v>132</v>
       </c>
       <c r="B168">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
@@ -3107,7 +3112,7 @@
         <v>136</v>
       </c>
       <c r="B173">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
@@ -3123,7 +3128,7 @@
         <v>137</v>
       </c>
       <c r="B175">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
@@ -3163,7 +3168,7 @@
         <v>142</v>
       </c>
       <c r="B180">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
@@ -3187,7 +3192,7 @@
         <v>145</v>
       </c>
       <c r="B183">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
@@ -3243,7 +3248,7 @@
         <v>151</v>
       </c>
       <c r="B190">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
@@ -3275,7 +3280,7 @@
         <v>153</v>
       </c>
       <c r="B194">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
@@ -3331,7 +3336,7 @@
         <v>160</v>
       </c>
       <c r="B201">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
@@ -3355,7 +3360,7 @@
         <v>163</v>
       </c>
       <c r="B204">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
@@ -3395,7 +3400,7 @@
         <v>167</v>
       </c>
       <c r="B209">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.3">
@@ -3459,7 +3464,7 @@
         <v>173</v>
       </c>
       <c r="B217">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
@@ -3483,7 +3488,7 @@
         <v>176</v>
       </c>
       <c r="B220">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.3">
@@ -3531,7 +3536,7 @@
         <v>181</v>
       </c>
       <c r="B226">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.3">
@@ -3547,7 +3552,7 @@
         <v>182</v>
       </c>
       <c r="B228">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
@@ -3563,7 +3568,7 @@
         <v>184</v>
       </c>
       <c r="B230">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
@@ -3611,7 +3616,7 @@
         <v>189</v>
       </c>
       <c r="B236">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
@@ -3619,7 +3624,7 @@
         <v>190</v>
       </c>
       <c r="B237">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
@@ -3627,7 +3632,7 @@
         <v>191</v>
       </c>
       <c r="B238">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.3">
@@ -3675,7 +3680,7 @@
         <v>195</v>
       </c>
       <c r="B244">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
@@ -3723,7 +3728,7 @@
         <v>199</v>
       </c>
       <c r="B250">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
@@ -3731,7 +3736,7 @@
         <v>200</v>
       </c>
       <c r="B251">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
@@ -3747,7 +3752,7 @@
         <v>202</v>
       </c>
       <c r="B253">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.3">
@@ -3755,7 +3760,7 @@
         <v>203</v>
       </c>
       <c r="B254">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.3">
@@ -3763,7 +3768,7 @@
         <v>204</v>
       </c>
       <c r="B255">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.3">
@@ -3803,7 +3808,7 @@
         <v>207</v>
       </c>
       <c r="B260">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.3">
@@ -3811,7 +3816,7 @@
         <v>208</v>
       </c>
       <c r="B261">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.3">
@@ -3851,7 +3856,7 @@
         <v>211</v>
       </c>
       <c r="B266">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.3">
@@ -3907,7 +3912,7 @@
         <v>216</v>
       </c>
       <c r="B273">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.3">
@@ -3947,7 +3952,7 @@
         <v>221</v>
       </c>
       <c r="B278">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.3">
@@ -4011,7 +4016,7 @@
         <v>226</v>
       </c>
       <c r="B286">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.3">
@@ -4027,7 +4032,7 @@
         <v>227</v>
       </c>
       <c r="B288">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.3">
@@ -4043,7 +4048,7 @@
         <v>229</v>
       </c>
       <c r="B290">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.3">
@@ -4059,7 +4064,7 @@
         <v>231</v>
       </c>
       <c r="B292">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.3">
@@ -4067,7 +4072,7 @@
         <v>232</v>
       </c>
       <c r="B293">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.3">
@@ -4075,7 +4080,7 @@
         <v>233</v>
       </c>
       <c r="B294">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.3">
@@ -4099,7 +4104,7 @@
         <v>236</v>
       </c>
       <c r="B297">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.3">
@@ -4107,7 +4112,7 @@
         <v>237</v>
       </c>
       <c r="B298">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.3">
@@ -4147,8 +4152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="B201" sqref="B201"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="B190" sqref="B190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4230,7 +4235,7 @@
         <v>246</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -4286,7 +4291,7 @@
         <v>253</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -4302,7 +4307,7 @@
         <v>255</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -4326,7 +4331,7 @@
         <v>258</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -4342,7 +4347,7 @@
         <v>260</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -4358,7 +4363,7 @@
         <v>262</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -4382,7 +4387,7 @@
         <v>265</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -4438,7 +4443,7 @@
         <v>267</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -4454,7 +4459,7 @@
         <v>269</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -4478,7 +4483,7 @@
         <v>271</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -4574,7 +4579,7 @@
         <v>278</v>
       </c>
       <c r="B53">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -4638,7 +4643,7 @@
         <v>283</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
@@ -4654,7 +4659,7 @@
         <v>285</v>
       </c>
       <c r="B63">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
@@ -4678,7 +4683,7 @@
         <v>288</v>
       </c>
       <c r="B66">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
@@ -4702,7 +4707,7 @@
         <v>290</v>
       </c>
       <c r="B69">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
@@ -4710,7 +4715,7 @@
         <v>291</v>
       </c>
       <c r="B70">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
@@ -4726,7 +4731,7 @@
         <v>293</v>
       </c>
       <c r="B72">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
@@ -4742,7 +4747,7 @@
         <v>295</v>
       </c>
       <c r="B74">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
@@ -4750,7 +4755,7 @@
         <v>296</v>
       </c>
       <c r="B75">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
@@ -4790,7 +4795,7 @@
         <v>301</v>
       </c>
       <c r="B80">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
@@ -4814,7 +4819,7 @@
         <v>304</v>
       </c>
       <c r="B83">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
@@ -4838,7 +4843,7 @@
         <v>307</v>
       </c>
       <c r="B86">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
@@ -4878,7 +4883,7 @@
         <v>312</v>
       </c>
       <c r="B91">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
@@ -4910,7 +4915,7 @@
         <v>315</v>
       </c>
       <c r="B95">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
@@ -4934,7 +4939,7 @@
         <v>317</v>
       </c>
       <c r="B98">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
@@ -4982,7 +4987,7 @@
         <v>323</v>
       </c>
       <c r="B104">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
@@ -5006,7 +5011,7 @@
         <v>325</v>
       </c>
       <c r="B107">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
@@ -5014,7 +5019,7 @@
         <v>326</v>
       </c>
       <c r="B108">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
@@ -5046,7 +5051,7 @@
         <v>329</v>
       </c>
       <c r="B112">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
@@ -5062,7 +5067,7 @@
         <v>331</v>
       </c>
       <c r="B114">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
@@ -5086,7 +5091,7 @@
         <v>332</v>
       </c>
       <c r="B117">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
@@ -5094,7 +5099,7 @@
         <v>333</v>
       </c>
       <c r="B118">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
@@ -5102,7 +5107,7 @@
         <v>334</v>
       </c>
       <c r="B119">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
@@ -5110,7 +5115,7 @@
         <v>335</v>
       </c>
       <c r="B120">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
@@ -5118,7 +5123,7 @@
         <v>336</v>
       </c>
       <c r="B121">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
@@ -5166,7 +5171,7 @@
         <v>339</v>
       </c>
       <c r="B127">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
@@ -5174,7 +5179,7 @@
         <v>340</v>
       </c>
       <c r="B128">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
@@ -5198,7 +5203,7 @@
         <v>343</v>
       </c>
       <c r="B131">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
@@ -5222,7 +5227,7 @@
         <v>345</v>
       </c>
       <c r="B134">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
@@ -5230,7 +5235,7 @@
         <v>346</v>
       </c>
       <c r="B135">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
@@ -5254,7 +5259,7 @@
         <v>348</v>
       </c>
       <c r="B138">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
@@ -5262,7 +5267,7 @@
         <v>349</v>
       </c>
       <c r="B139">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
@@ -5270,7 +5275,7 @@
         <v>350</v>
       </c>
       <c r="B140">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
@@ -5310,7 +5315,7 @@
         <v>353</v>
       </c>
       <c r="B145">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
@@ -5350,7 +5355,7 @@
         <v>355</v>
       </c>
       <c r="B150">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
@@ -5366,7 +5371,7 @@
         <v>357</v>
       </c>
       <c r="B152">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
@@ -5374,7 +5379,7 @@
         <v>358</v>
       </c>
       <c r="B153">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
@@ -5390,7 +5395,7 @@
         <v>360</v>
       </c>
       <c r="B155">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
@@ -5406,7 +5411,7 @@
         <v>361</v>
       </c>
       <c r="B157">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
@@ -5414,7 +5419,7 @@
         <v>362</v>
       </c>
       <c r="B158">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
@@ -5430,7 +5435,7 @@
         <v>364</v>
       </c>
       <c r="B160">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
@@ -5454,7 +5459,7 @@
         <v>367</v>
       </c>
       <c r="B163">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
@@ -5470,7 +5475,7 @@
         <v>369</v>
       </c>
       <c r="B165">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
@@ -5486,7 +5491,7 @@
         <v>371</v>
       </c>
       <c r="B167">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
@@ -5534,7 +5539,7 @@
         <v>375</v>
       </c>
       <c r="B173">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
@@ -5542,7 +5547,7 @@
         <v>376</v>
       </c>
       <c r="B174">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
@@ -5574,7 +5579,7 @@
         <v>380</v>
       </c>
       <c r="B178">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
@@ -5622,7 +5627,7 @@
         <v>385</v>
       </c>
       <c r="B184">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
@@ -5670,7 +5675,7 @@
         <v>390</v>
       </c>
       <c r="B190">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
@@ -5678,7 +5683,7 @@
         <v>391</v>
       </c>
       <c r="B191">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
@@ -5686,7 +5691,7 @@
         <v>392</v>
       </c>
       <c r="B192">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
@@ -5710,7 +5715,7 @@
         <v>394</v>
       </c>
       <c r="B195">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
@@ -5742,7 +5747,7 @@
         <v>397</v>
       </c>
       <c r="B199">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>